<commit_message>
toevoegen van nieuwe vragen
</commit_message>
<xml_diff>
--- a/druppelkiezer.xlsx
+++ b/druppelkiezer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071D9516-B12A-4514-B9FD-979C00D56572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91D33B3-D323-439E-8640-CFF4F161B253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="158">
   <si>
     <t>naam</t>
   </si>
@@ -437,13 +437,76 @@
   </si>
   <si>
     <t>if (1=='nee' &amp;&amp; 2=='nee' &amp;&amp; 3=='nee' &amp;&amp; 4 == 'nee' &amp;&amp; 5 == 'nee' &amp;&amp; 6 == 'nee' &amp;&amp; 7 == 'nee'){'je blijkt nergens last van te hebben: fijn voor jou! Bedankt voor je bezoek'}else{10}</t>
+  </si>
+  <si>
+    <t>kun je vertellen hoeveel keer je klachten voorkomen in een maand?</t>
+  </si>
+  <si>
+    <t>slechts enkele keren per maand</t>
+  </si>
+  <si>
+    <t>1 à 2 keer per week</t>
+  </si>
+  <si>
+    <t>3 à 5 keer per week (zo goed als) dagelijk</t>
+  </si>
+  <si>
+    <t>lipiden</t>
+  </si>
+  <si>
+    <t>Wanneer begin je meestal last te krijgen?</t>
+  </si>
+  <si>
+    <t>s avonds na het uithalen van mijn contactlenzen</t>
+  </si>
+  <si>
+    <t>s avonds</t>
+  </si>
+  <si>
+    <t>in de latere namiddag</t>
+  </si>
+  <si>
+    <t>al van rond de middag</t>
+  </si>
+  <si>
+    <t>in de loop van de ochtend</t>
+  </si>
+  <si>
+    <t>van bij het opstaan al</t>
+  </si>
+  <si>
+    <t>mijn klasse: bevat 1</t>
+  </si>
+  <si>
+    <t>mijn klasse: bevat 2</t>
+  </si>
+  <si>
+    <t>mijn klasse: bevat 3</t>
+  </si>
+  <si>
+    <t>mijn klasse: bevat 4</t>
+  </si>
+  <si>
+    <t>ooit laten krassen of laseren: slechte traanhechting, snelle verdamping</t>
+  </si>
+  <si>
+    <t>bepaalde ziektes: Sjögren, aangezichtsverlamming</t>
+  </si>
+  <si>
+    <t>tranen je ogen als je op een koude ochtend in de wind loopt?</t>
+  </si>
+  <si>
+    <t>hangen de onderste oogleden een beetje? Ectropion</t>
+  </si>
+  <si>
+    <t>MGD: blokkage en retractie Meibomklier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +533,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -550,6 +619,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -864,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08721AE2-DE19-4E70-9717-105832BF9954}">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +951,7 @@
     <col min="12" max="15" width="4.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,8 +997,11 @@
       <c r="O1" s="17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -955,8 +1029,9 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="15"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -992,8 +1067,9 @@
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1031,8 +1107,9 @@
       </c>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1066,8 +1143,9 @@
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="15"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1111,8 +1189,11 @@
       <c r="O6" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1154,8 +1235,9 @@
       <c r="O7" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1191,8 +1273,9 @@
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1226,8 +1309,9 @@
       </c>
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="15"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1259,8 +1343,9 @@
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1290,8 +1375,9 @@
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1323,8 +1409,9 @@
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="15"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1360,8 +1447,9 @@
       <c r="O13" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="15"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1397,8 +1485,9 @@
       <c r="O14" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="15"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1434,8 +1523,9 @@
       <c r="O15" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1471,8 +1561,9 @@
       </c>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1512,8 +1603,9 @@
       <c r="O17" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1539,8 +1631,9 @@
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1570,8 +1663,9 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="15"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1585,7 +1679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1599,7 +1693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1613,7 +1707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1627,7 +1721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1641,7 +1735,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1655,7 +1749,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -2146,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DC6708-B8A1-4658-896A-91A64A86E2C2}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,8 +2760,8 @@
       <c r="C47" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="16" t="s">
-        <v>134</v>
+      <c r="D47" s="16">
+        <v>30</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>132</v>
@@ -2681,19 +2775,412 @@
       <c r="C48" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D48" s="16" t="s">
-        <v>134</v>
+      <c r="D48" s="16">
+        <v>30</v>
       </c>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>30</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>30</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="18">
+        <v>40</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>30</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="18">
+        <v>40</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>30</v>
+      </c>
+      <c r="B53" s="15"/>
+      <c r="C53" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" s="18">
+        <v>40</v>
+      </c>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>40</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>40</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="18">
+        <v>52</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>40</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" s="18">
+        <v>52</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>40</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="18">
+        <v>52</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>40</v>
+      </c>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="18">
+        <v>52</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>40</v>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D60" s="18">
+        <v>52</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>40</v>
+      </c>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="18">
+        <v>52</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>52</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>52</v>
+      </c>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="18">
+        <v>54</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>52</v>
+      </c>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="18">
+        <v>54</v>
+      </c>
+      <c r="E65" s="18"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>54</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>54</v>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="18">
+        <v>58</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>54</v>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="18">
+        <v>58</v>
+      </c>
+      <c r="E69" s="18"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
+        <v>58</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
+        <v>58</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="18">
+        <v>59</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
+        <v>58</v>
+      </c>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" s="18">
+        <v>59</v>
+      </c>
+      <c r="E73" s="18"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
+        <v>59</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
+        <v>59</v>
+      </c>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="18">
+        <v>60</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="15">
+        <v>59</v>
+      </c>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" s="18">
+        <v>60</v>
+      </c>
+      <c r="E77" s="18"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15">
+        <v>60</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="15">
+        <v>60</v>
+      </c>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="15">
+        <v>60</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="18"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
toevoegen achtergrond + progressbar
</commit_message>
<xml_diff>
--- a/druppelkiezer.xlsx
+++ b/druppelkiezer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91D33B3-D323-439E-8640-CFF4F161B253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0582A7DD-523E-41EA-9865-DEDCA4CC8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="159">
   <si>
     <t>naam</t>
   </si>
@@ -385,45 +385,15 @@
     <t>vervolg</t>
   </si>
   <si>
-    <t>voelen je ogen droog aan?</t>
-  </si>
-  <si>
-    <t>voelen je ogen vermoeid aan?</t>
-  </si>
-  <si>
-    <t>schurend gevoel</t>
-  </si>
-  <si>
-    <t>branderig gevoel</t>
-  </si>
-  <si>
-    <t>geïrriteerde ogen, prikken</t>
-  </si>
-  <si>
-    <t>jeukende ogen</t>
-  </si>
-  <si>
     <t>nee, ik heb deze klachten ongeacht waar ik ben</t>
   </si>
   <si>
     <t>verpakking</t>
   </si>
   <si>
-    <t>klachten bij kijken naar schermen, … of ook bij langdurig lezen</t>
-  </si>
-  <si>
     <t>ik heb deze klachten ongeacht wat ik aan het doen ben</t>
   </si>
   <si>
-    <t>klachten tgv airco, verwarming, droge lucht, warmte?</t>
-  </si>
-  <si>
-    <t>klachten bij wind, tocht, …</t>
-  </si>
-  <si>
-    <t>klachten als je in een stofferige of vuile omgeving bent?</t>
-  </si>
-  <si>
     <t>stof/vervuiling</t>
   </si>
   <si>
@@ -439,9 +409,6 @@
     <t>if (1=='nee' &amp;&amp; 2=='nee' &amp;&amp; 3=='nee' &amp;&amp; 4 == 'nee' &amp;&amp; 5 == 'nee' &amp;&amp; 6 == 'nee' &amp;&amp; 7 == 'nee'){'je blijkt nergens last van te hebben: fijn voor jou! Bedankt voor je bezoek'}else{10}</t>
   </si>
   <si>
-    <t>kun je vertellen hoeveel keer je klachten voorkomen in een maand?</t>
-  </si>
-  <si>
     <t>slechts enkele keren per maand</t>
   </si>
   <si>
@@ -454,9 +421,6 @@
     <t>lipiden</t>
   </si>
   <si>
-    <t>Wanneer begin je meestal last te krijgen?</t>
-  </si>
-  <si>
     <t>s avonds na het uithalen van mijn contactlenzen</t>
   </si>
   <si>
@@ -487,19 +451,58 @@
     <t>mijn klasse: bevat 4</t>
   </si>
   <si>
-    <t>ooit laten krassen of laseren: slechte traanhechting, snelle verdamping</t>
-  </si>
-  <si>
-    <t>bepaalde ziektes: Sjögren, aangezichtsverlamming</t>
-  </si>
-  <si>
-    <t>tranen je ogen als je op een koude ochtend in de wind loopt?</t>
-  </si>
-  <si>
-    <t>hangen de onderste oogleden een beetje? Ectropion</t>
-  </si>
-  <si>
-    <t>MGD: blokkage en retractie Meibomklier</t>
+    <t>Voelen uw ogen droog aan?</t>
+  </si>
+  <si>
+    <t>Voelen uw ogen vermoeid aan?</t>
+  </si>
+  <si>
+    <t>Heeft u last van een branderig gevoel?</t>
+  </si>
+  <si>
+    <t>Heeft u last van een schurend gevoel?</t>
+  </si>
+  <si>
+    <t>Heeft u geïrriteerde/prikkende ogen?</t>
+  </si>
+  <si>
+    <t>Heeft u last van rode ogen?</t>
+  </si>
+  <si>
+    <t>Heeft u jeukende ogen?</t>
+  </si>
+  <si>
+    <t>Heeft u klachten bij kijken naar schermen, … of ook bij langdurig lezen?</t>
+  </si>
+  <si>
+    <t>Heeft u klachten t.g.v. airco, verwarming, droge lucht of warmte?</t>
+  </si>
+  <si>
+    <t>Heeft u klachten als u in een stofferige of vuile omgeving bent?</t>
+  </si>
+  <si>
+    <t>Wanneer begint u meestal last te krijgen?</t>
+  </si>
+  <si>
+    <t>Tranen uw ogen als u op een koude ochtend in de wind loopt?</t>
+  </si>
+  <si>
+    <t>Hangen uw onderste oogleden een beetje? (Ectropion)</t>
+  </si>
+  <si>
+    <t>Heeft u last van MGD? (blokkage en retractie Meibomklier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heeft u klachten bij wind, tocht, … ? </t>
+  </si>
+  <si>
+    <t>Kunt u vertellen hoeveel keer uw klachten voorkomen in een maand?</t>
+  </si>
+  <si>
+    <t>Heeft u uw ogen ooit laten krassen of laseren? (slechte traanhechting, snelle verdamping)</t>
+  </si>
+  <si>
+    <t>Heeft u bepaalde ziektes?  (Sjögren, aangezichtsverlamming)</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -619,8 +622,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -938,7 +940,7 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -998,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2242,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DC6708-B8A1-4658-896A-91A64A86E2C2}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +2274,7 @@
         <v>118</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2280,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2326,7 +2328,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2356,7 +2358,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E8" s="9"/>
     </row>
@@ -2372,7 +2374,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2411,7 +2413,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2450,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2496,7 +2498,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2542,7 +2544,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2572,7 +2574,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E26" s="8"/>
     </row>
@@ -2608,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -2635,7 +2637,7 @@
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D36" s="16">
         <v>11</v>
@@ -2654,7 +2656,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -2681,7 +2683,7 @@
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D40" s="16">
         <v>12</v>
@@ -2700,7 +2702,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -2727,7 +2729,7 @@
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D44" s="16">
         <v>18</v>
@@ -2746,7 +2748,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -2764,7 +2766,7 @@
         <v>30</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2773,7 +2775,7 @@
       </c>
       <c r="B48" s="16"/>
       <c r="C48" s="16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D48" s="16">
         <v>30</v>
@@ -2791,8 +2793,8 @@
       <c r="A50" s="15">
         <v>30</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>137</v>
+      <c r="B50" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -2803,13 +2805,13 @@
         <v>30</v>
       </c>
       <c r="B51" s="15"/>
-      <c r="C51" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D51" s="18">
+      <c r="C51" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="16">
         <v>40</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E51" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2819,12 +2821,12 @@
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D52" s="18">
+        <v>128</v>
+      </c>
+      <c r="D52" s="16">
         <v>40</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E52" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2833,10 +2835,10 @@
         <v>30</v>
       </c>
       <c r="B53" s="15"/>
-      <c r="C53" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D53" s="18">
+      <c r="C53" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="16">
         <v>40</v>
       </c>
       <c r="E53" s="15"/>
@@ -2852,332 +2854,332 @@
       <c r="A55" s="15">
         <v>40</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
+      <c r="B55" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>40</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" s="18">
+      <c r="B56" s="16"/>
+      <c r="C56" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="16">
         <v>52</v>
       </c>
-      <c r="E56" s="18" t="s">
-        <v>149</v>
+      <c r="E56" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>40</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D57" s="18">
+      <c r="B57" s="16"/>
+      <c r="C57" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" s="16">
         <v>52</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>150</v>
+      <c r="E57" s="16" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>40</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="18">
+      <c r="B58" s="16"/>
+      <c r="C58" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" s="16">
         <v>52</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>150</v>
+      <c r="E58" s="16" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>40</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D59" s="18">
+      <c r="B59" s="16"/>
+      <c r="C59" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="16">
         <v>52</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>151</v>
+      <c r="E59" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>40</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="18">
+      <c r="B60" s="16"/>
+      <c r="C60" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="16">
         <v>52</v>
       </c>
-      <c r="E60" s="18" t="s">
-        <v>151</v>
+      <c r="E60" s="16" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>40</v>
       </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" s="18">
+      <c r="B61" s="16"/>
+      <c r="C61" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="16">
         <v>52</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>152</v>
+      <c r="E61" s="16" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>52</v>
       </c>
-      <c r="B63" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
+      <c r="B63" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>52</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="18">
+      <c r="B64" s="16"/>
+      <c r="C64" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="16">
         <v>54</v>
       </c>
-      <c r="E64" s="18" t="s">
-        <v>141</v>
+      <c r="E64" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>52</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18" t="s">
+      <c r="B65" s="16"/>
+      <c r="C65" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="18">
+      <c r="D65" s="16">
         <v>54</v>
       </c>
-      <c r="E65" s="18"/>
+      <c r="E65" s="16"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>54</v>
       </c>
-      <c r="B67" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
+      <c r="B67" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>54</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68" s="18">
+      <c r="B68" s="16"/>
+      <c r="C68" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="16">
         <v>58</v>
       </c>
-      <c r="E68" s="18" t="s">
-        <v>141</v>
+      <c r="E68" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>54</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18" t="s">
+      <c r="B69" s="16"/>
+      <c r="C69" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D69" s="18">
+      <c r="D69" s="16">
         <v>58</v>
       </c>
-      <c r="E69" s="18"/>
+      <c r="E69" s="16"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>58</v>
       </c>
-      <c r="B71" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
+      <c r="B71" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>58</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" s="18">
+      <c r="B72" s="16"/>
+      <c r="C72" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="16">
         <v>59</v>
       </c>
-      <c r="E72" s="18" t="s">
-        <v>141</v>
+      <c r="E72" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>58</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18" t="s">
+      <c r="B73" s="16"/>
+      <c r="C73" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="18">
+      <c r="D73" s="16">
         <v>59</v>
       </c>
-      <c r="E73" s="18"/>
+      <c r="E73" s="16"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>59</v>
       </c>
-      <c r="B75" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
+      <c r="B75" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>59</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="18">
+      <c r="B76" s="16"/>
+      <c r="C76" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="16">
         <v>60</v>
       </c>
-      <c r="E76" s="18" t="s">
-        <v>141</v>
+      <c r="E76" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>59</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18" t="s">
+      <c r="B77" s="16"/>
+      <c r="C77" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D77" s="18">
+      <c r="D77" s="16">
         <v>60</v>
       </c>
-      <c r="E77" s="18"/>
+      <c r="E77" s="16"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>60</v>
       </c>
-      <c r="B79" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
+      <c r="B79" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>60</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>141</v>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>60</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18" t="s">
+      <c r="B81" s="16"/>
+      <c r="C81" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E81" s="18"/>
+      <c r="D81" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E81" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
aanpassen vraag 30 en 40 + toevoegen van ampullen/houdbaarheid + mijn klasse
</commit_message>
<xml_diff>
--- a/druppelkiezer.xlsx
+++ b/druppelkiezer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0582A7DD-523E-41EA-9865-DEDCA4CC8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE78891-7C2D-47BD-8D45-AE2786957E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="171">
   <si>
     <t>naam</t>
   </si>
@@ -415,9 +415,6 @@
     <t>1 à 2 keer per week</t>
   </si>
   <si>
-    <t>3 à 5 keer per week (zo goed als) dagelijk</t>
-  </si>
-  <si>
     <t>lipiden</t>
   </si>
   <si>
@@ -503,6 +500,45 @@
   </si>
   <si>
     <t>Heeft u bepaalde ziektes?  (Sjögren, aangezichtsverlamming)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 à 5 keer per week </t>
+  </si>
+  <si>
+    <t>(zo goed als) dagelijks</t>
+  </si>
+  <si>
+    <t>er valt geen lijn in te trekken, het is random, wisselvallig</t>
+  </si>
+  <si>
+    <t>houdbaarheid</t>
+  </si>
+  <si>
+    <t>nvt</t>
+  </si>
+  <si>
+    <t>ampullen OF 6mnd</t>
+  </si>
+  <si>
+    <t>6mnd</t>
+  </si>
+  <si>
+    <t>2mnd</t>
+  </si>
+  <si>
+    <t>3mnd</t>
+  </si>
+  <si>
+    <t>2;3</t>
+  </si>
+  <si>
+    <t>mijnKlasse</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>3;4</t>
   </si>
 </sst>
 </file>
@@ -585,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -623,6 +659,7 @@
       <alignment horizontal="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -937,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08721AE2-DE19-4E70-9717-105832BF9954}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +990,7 @@
     <col min="12" max="15" width="4.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1000,10 +1037,16 @@
         <v>12</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1032,8 +1075,14 @@
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1070,8 +1119,14 @@
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R3" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1110,8 +1165,14 @@
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1146,8 +1207,14 @@
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1194,8 +1261,14 @@
       <c r="P6" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1238,8 +1311,14 @@
         <v>18</v>
       </c>
       <c r="P7" s="15"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1276,8 +1355,14 @@
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1312,8 +1397,14 @@
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="R9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1346,8 +1437,14 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
       <c r="P10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1378,8 +1475,14 @@
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
       <c r="P11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1412,8 +1515,14 @@
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1450,8 +1559,14 @@
         <v>18</v>
       </c>
       <c r="P13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R13" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1488,8 +1603,12 @@
         <v>18</v>
       </c>
       <c r="P14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R14" s="15"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1526,8 +1645,12 @@
         <v>18</v>
       </c>
       <c r="P15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="R15" s="15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1564,8 +1687,14 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R16" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1606,8 +1735,14 @@
         <v>18</v>
       </c>
       <c r="P17" s="15"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1634,8 +1769,12 @@
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1666,8 +1805,10 @@
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1681,7 +1822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1695,7 +1836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1709,7 +1850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1723,7 +1864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1737,7 +1878,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1751,7 +1892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -2236,16 +2377,17 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DC6708-B8A1-4658-896A-91A64A86E2C2}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2328,7 +2470,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2374,7 +2516,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2413,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -2452,7 +2594,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2498,7 +2640,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2544,7 +2686,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2610,7 +2752,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -2656,7 +2798,7 @@
         <v>11</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -2702,7 +2844,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -2748,7 +2890,7 @@
         <v>18</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -2794,7 +2936,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -2812,7 +2954,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,7 +2969,7 @@
         <v>40</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,7 +2978,7 @@
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="16" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="D53" s="16">
         <v>40</v>
@@ -2844,37 +2986,35 @@
       <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="15">
+        <v>30</v>
+      </c>
       <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
+      <c r="C54" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="16">
+        <v>40</v>
+      </c>
       <c r="E54" s="15"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
-        <v>40</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>40</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" s="16">
-        <v>52</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>137</v>
-      </c>
+      <c r="B56" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
@@ -2882,13 +3022,13 @@
       </c>
       <c r="B57" s="16"/>
       <c r="C57" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D57" s="16">
         <v>52</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2896,14 +3036,14 @@
         <v>40</v>
       </c>
       <c r="B58" s="16"/>
-      <c r="C58" s="16" t="s">
-        <v>133</v>
+      <c r="C58" s="18" t="s">
+        <v>131</v>
       </c>
       <c r="D58" s="16">
         <v>52</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2912,13 +3052,13 @@
       </c>
       <c r="B59" s="16"/>
       <c r="C59" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D59" s="16">
         <v>52</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2927,13 +3067,13 @@
       </c>
       <c r="B60" s="16"/>
       <c r="C60" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D60" s="16">
         <v>52</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,244 +3082,274 @@
       </c>
       <c r="B61" s="16"/>
       <c r="C61" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D61" s="16">
         <v>52</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="15">
+        <v>40</v>
+      </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+      <c r="C62" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D62" s="16">
+        <v>52</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
+        <v>40</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D63" s="19">
         <v>52</v>
       </c>
-      <c r="B63" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
+      <c r="E63" s="19" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="15">
-        <v>52</v>
-      </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="16">
-        <v>54</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>52</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" s="16">
+      <c r="B65" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>52</v>
+      </c>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="16">
         <v>54</v>
       </c>
-      <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
+      <c r="E66" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
+        <v>52</v>
+      </c>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="16">
         <v>54</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
       <c r="E67" s="16"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="15">
-        <v>54</v>
-      </c>
+      <c r="A68" s="15"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68" s="16">
-        <v>58</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>54</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="16">
+      <c r="B69" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
+        <v>54</v>
+      </c>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="16">
         <v>58</v>
       </c>
-      <c r="E69" s="16"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
+      <c r="E70" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
+        <v>54</v>
+      </c>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" s="16">
         <v>58</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
       <c r="E71" s="16"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="15">
-        <v>58</v>
-      </c>
+      <c r="A72" s="15"/>
       <c r="B72" s="16"/>
-      <c r="C72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" s="16">
-        <v>59</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>58</v>
       </c>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="16">
+      <c r="B73" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
+        <v>58</v>
+      </c>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="16">
         <v>59</v>
       </c>
-      <c r="E73" s="16"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
+      <c r="E74" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
+        <v>58</v>
+      </c>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" s="16">
         <v>59</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
       <c r="E75" s="16"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="15">
-        <v>59</v>
-      </c>
+      <c r="A76" s="15"/>
       <c r="B76" s="16"/>
-      <c r="C76" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="16">
-        <v>60</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>59</v>
       </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" s="16">
+      <c r="B77" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15">
+        <v>59</v>
+      </c>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="16">
         <v>60</v>
       </c>
-      <c r="E77" s="16"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
+      <c r="E78" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
+        <v>59</v>
+      </c>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="16">
         <v>60</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
       <c r="E79" s="16"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="15">
-        <v>60</v>
-      </c>
+      <c r="A80" s="15"/>
       <c r="B80" s="16"/>
-      <c r="C80" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>60</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16" t="s">
+      <c r="B81" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="15">
+        <v>60</v>
+      </c>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
+        <v>60</v>
+      </c>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D83" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="E81" s="16"/>
+      <c r="E83" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
aanpassing aan excel file
</commit_message>
<xml_diff>
--- a/druppelkiezer.xlsx
+++ b/druppelkiezer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\lens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE78891-7C2D-47BD-8D45-AE2786957E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E45FD56-7A5D-4875-9D40-887A2D998638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF2FD3AD-E9A5-4ED3-883E-3545DB377DF1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="172">
   <si>
     <t>naam</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>3;4</t>
+  </si>
+  <si>
+    <t>1mnd</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -659,7 +662,6 @@
       <alignment horizontal="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -977,7 +979,7 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1608,9 @@
       <c r="Q14" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="R14" s="15"/>
+      <c r="R14" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1648,7 +1652,9 @@
       <c r="Q15" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="R15" s="15"/>
+      <c r="R15" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1772,7 +1778,9 @@
       <c r="Q18" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="R18" s="15"/>
+      <c r="R18" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1805,8 +1813,12 @@
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
+      <c r="Q19" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -3111,13 +3123,13 @@
         <v>40</v>
       </c>
       <c r="B63" s="15"/>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D63" s="19">
+      <c r="D63" s="16">
         <v>52</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="16" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>